<commit_message>
Fix on extension 39d2715b0810ca12a7e42ab2f151ee77d64dfe30
</commit_message>
<xml_diff>
--- a/feature/cpts/ig/StructureDefinition-sas-cpts-slot-aggregator.xlsx
+++ b/feature/cpts/ig/StructureDefinition-sas-cpts-slot-aggregator.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-28T14:23:52+00:00</t>
+    <t>2024-06-03T14:45:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -885,7 +885,7 @@
     <t>Slot.schedule</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/sas/StructureDefinition/sas-sos-schedule-aggregator)
+    <t xml:space="preserve">Reference(http://sas.fr/fhir/StructureDefinition/FrScheduleAgregateur)
 </t>
   </si>
   <si>

</xml_diff>